<commit_message>
Thêm ppt Báo cáo 1
</commit_message>
<xml_diff>
--- a/Documents/Ma Trận Chức Năng.xlsx
+++ b/Documents/Ma Trận Chức Năng.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\LuanVan-2-5\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://balastechnologiescom-my.sharepoint.com/personal/baonh_balastechnologies_com/Documents/LUẬN VĂN/office-space-rental/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7459D734-0830-446A-9317-CEF64BE7FE48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{7459D734-0830-446A-9317-CEF64BE7FE48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D558EF57-1495-4A88-998F-AB06F90249C5}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$G$40</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="45">
   <si>
     <t>Chức năng</t>
   </si>
@@ -237,6 +240,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -526,527 +533,527 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="B1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="56.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="56.5234375" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" customWidth="1"/>
+    <col min="4" max="4" width="19.5234375" customWidth="1"/>
+    <col min="5" max="5" width="14.83984375" customWidth="1"/>
+    <col min="6" max="6" width="14.5234375" customWidth="1"/>
+    <col min="7" max="7" width="13.9453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="2" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B11" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B12" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B14" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>43</v>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B15" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="3"/>
+      <c r="G15" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B17" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="C17" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>43</v>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B18" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B19" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="C19" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="3"/>
+      <c r="F22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B23" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>43</v>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B24" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="E24" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B28" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
+      <c r="C28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B29" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B30" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
+      <c r="C30" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B31" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
+      <c r="C31" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B32" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
+      <c r="C32" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B33" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34" s="3"/>
+      <c r="F33" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B34" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C34" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D35" s="3"/>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B35" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B36" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B37" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
+      <c r="C37" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G37" s="3"/>
+    </row>
+    <row r="38" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B38" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F37" s="3"/>
-    </row>
-    <row r="38" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
+      <c r="C38" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G38" s="3"/>
+    </row>
+    <row r="39" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B39" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-    </row>
-    <row r="39" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C39" s="3"/>
+      <c r="C39" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="B2:G40" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Thêm chức năng searchOS_Lessee
</commit_message>
<xml_diff>
--- a/Documents/Ma Trận Chức Năng.xlsx
+++ b/Documents/Ma Trận Chức Năng.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://balastechnologiescom-my.sharepoint.com/personal/baonh_balastechnologies_com/Documents/LUẬN VĂN/office-space-rental/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://balastechnologiescom-my.sharepoint.com/personal/baonh_balastechnologies_com/Documents/THESIS/office-space-rental/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{7459D734-0830-446A-9317-CEF64BE7FE48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D558EF57-1495-4A88-998F-AB06F90249C5}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{7459D734-0830-446A-9317-CEF64BE7FE48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61BC2B23-C23D-454B-9868-85B387DA8040}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -181,12 +181,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -216,13 +222,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -240,10 +250,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -536,7 +542,7 @@
   <dimension ref="B1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -979,13 +985,13 @@
       <c r="G35" s="3"/>
     </row>
     <row r="36" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36" s="3" t="s">
+      <c r="C36" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E36" s="3"/>
@@ -993,37 +999,37 @@
       <c r="G36" s="3"/>
     </row>
     <row r="37" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F37" s="3" t="s">
+      <c r="C37" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G37" s="3"/>
     </row>
     <row r="38" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F38" s="3" t="s">
+      <c r="C38" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G38" s="3"/>

</xml_diff>